<commit_message>
odds scraper, guts working... need to add the rest of the columns
</commit_message>
<xml_diff>
--- a/data/odds.xlsx
+++ b/data/odds.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="109">
   <si>
     <t xml:space="preserve">Index</t>
   </si>
@@ -31,18 +31,45 @@
     <t xml:space="preserve">Team 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Team 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Saturday, August 24</t>
   </si>
   <si>
     <t xml:space="preserve">Florida State Seminoles</t>
   </si>
   <si>
+    <t xml:space="preserve">Georgia Tech Yellow Jackets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMU Mustangs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nevada Wolf Pack</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thursday, August 29</t>
   </si>
   <si>
     <t xml:space="preserve">North Carolina Tar Heels</t>
   </si>
   <si>
+    <t xml:space="preserve">Minnesota Golden Gophers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Dakota Fighting Hawks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colorado Buffaloes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coastal Carolina Chanticleers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jacksonville State Gamecocks</t>
+  </si>
+  <si>
     <t xml:space="preserve">Friday, August 30</t>
   </si>
   <si>
@@ -52,28 +79,196 @@
     <t xml:space="preserve">Oklahoma Sooners</t>
   </si>
   <si>
+    <t xml:space="preserve">Florida Atlantic Owls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michigan State Spartans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Michigan Broncos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wisconsin-Eau Claire Blugolds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCU Horned Frogs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stanford Cardinal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Saturday, August 31</t>
   </si>
   <si>
     <t xml:space="preserve">Clemson Tigers</t>
   </si>
   <si>
-    <t xml:space="preserve">Texas A&amp;M-Commerce Lions</t>
-  </si>
-  <si>
     <t xml:space="preserve">Georgia Bulldogs</t>
   </si>
   <si>
+    <t xml:space="preserve">Virginia Tech Hokies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanderbilt Commodores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UConn Huskies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maryland Terrapins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penn State Nittany Lions</t>
+  </si>
+  <si>
     <t xml:space="preserve">West Virginia Mountaineers</t>
   </si>
   <si>
-    <t xml:space="preserve">Virginia Tech Hokies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vanderbilt Commodores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UConn Huskies</t>
+    <t xml:space="preserve">Kent State Golden Flashes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pittsburgh Panthers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southeast Missouri State Redhawks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oklahoma State Cowboys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miami Hurricanes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florida Gators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colorado State Rams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texas Longhorns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florida International Panthers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indiana Hoosiers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTEP Miners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nebraska Cornhuskers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akron Zips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Tennessee State Buccaneers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Michigan Eagles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massachusetts Minutemen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ohio Bobcats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syracuse Orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kennesaw State Owls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTSA Roadrunners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iowa Hawkeyes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boise State Broncos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Georgia Southern Eagles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old Dominion Monarchs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Carolina Gamecocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Texas Mean Green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Alabama Jaguars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Kentucky Hilltoppers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alabama Crimson Tide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNLV Rebels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Houston Cougars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sam Houston Bearkats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rice Owls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Troy Trojans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notre Dame Fighting Irish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texas A&amp;M Aggies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fresno State Bulldogs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michigan Wolverines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UCLA Bruins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hawaii Rainbow Warriors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Miss Golden Eagles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kentucky Wildcats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Georgia State Panthers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James Madison Dukes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charlotte 49ers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Mexico Lobos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arizona Wildcats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyoming Cowboys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arizona State Sun Devils</t>
   </si>
   <si>
     <t xml:space="preserve">Sunday, September 1</t>
@@ -82,6 +277,9 @@
     <t xml:space="preserve">USC Trojans</t>
   </si>
   <si>
+    <t xml:space="preserve">LSU Tigers</t>
+  </si>
+  <si>
     <t xml:space="preserve">Monday, September 2</t>
   </si>
   <si>
@@ -91,33 +289,39 @@
     <t xml:space="preserve">Saturday, September 7</t>
   </si>
   <si>
-    <t xml:space="preserve">Texas Longhorns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern Michigan Eagles</t>
+    <t xml:space="preserve">Iowa State Cyclones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tennessee Volunteers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC State Wolfpack</t>
   </si>
   <si>
     <t xml:space="preserve">Friday, September 13</t>
   </si>
   <si>
-    <t xml:space="preserve">Arizona Wildcats</t>
+    <t xml:space="preserve">Kansas State Wildcats</t>
   </si>
   <si>
     <t xml:space="preserve">Saturday, September 14</t>
   </si>
   <si>
-    <t xml:space="preserve">Alabama Crimson Tide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Penn State Nittany Lions</t>
+    <t xml:space="preserve">Oregon Ducks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oregon State Beavers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Washington State Cougars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Washington Huskies</t>
   </si>
   <si>
     <t xml:space="preserve">Saturday, September 21</t>
   </si>
   <si>
-    <t xml:space="preserve">NC State Wolfpack</t>
-  </si>
-  <si>
     <t xml:space="preserve">Friday, September 27</t>
   </si>
   <si>
@@ -127,31 +331,22 @@
     <t xml:space="preserve">Arkansas Razorbacks</t>
   </si>
   <si>
-    <t xml:space="preserve">St. Francis (PA) Red Flash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Texas A&amp;M Aggies</t>
+    <t xml:space="preserve">Louisville Cardinals</t>
   </si>
   <si>
     <t xml:space="preserve">Saturday, October 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Michigan Wolverines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern Washington Eagles</t>
-  </si>
-  <si>
     <t xml:space="preserve">Saturday, October 12</t>
   </si>
   <si>
-    <t xml:space="preserve">Jackson State Tigers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Tennessee State Buccaneers</t>
-  </si>
-  <si>
     <t xml:space="preserve">Saturday, October 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saturday, November 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ole Miss Rebels</t>
   </si>
 </sst>
 </file>
@@ -443,16 +638,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -465,16 +661,22 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -482,10 +684,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -493,10 +698,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,10 +712,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -515,10 +726,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,10 +740,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,10 +754,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -548,10 +768,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,10 +782,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -570,10 +796,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -581,10 +810,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -592,10 +824,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -603,10 +838,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>13</v>
+        <v>32</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,10 +852,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>13</v>
+        <v>34</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,10 +866,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>13</v>
+        <v>36</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,10 +880,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>14</v>
+        <v>38</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,10 +894,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>15</v>
+        <v>40</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,10 +908,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>15</v>
+        <v>42</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,10 +922,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,10 +936,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>15</v>
+        <v>46</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -691,10 +950,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>15</v>
+        <v>48</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,10 +964,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>16</v>
+        <v>50</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,10 +978,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>16</v>
+        <v>52</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,10 +992,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -735,10 +1006,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>16</v>
+        <v>55</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,10 +1020,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>16</v>
+        <v>57</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,10 +1034,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>12</v>
+        <v>59</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,10 +1048,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>17</v>
+        <v>61</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,10 +1062,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -790,10 +1076,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>17</v>
+        <v>65</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -801,10 +1090,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,10 +1104,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>21</v>
+        <v>68</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,10 +1118,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>23</v>
+        <v>70</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -834,10 +1132,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>23</v>
+        <v>72</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,10 +1146,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>24</v>
+        <v>74</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,7 +1163,10 @@
         <v>25</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>26</v>
+        <v>76</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -867,10 +1174,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>28</v>
+        <v>77</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,10 +1188,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>28</v>
+        <v>79</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,10 +1202,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>28</v>
+        <v>81</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -900,10 +1216,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>28</v>
+        <v>84</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -911,10 +1230,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>29</v>
+        <v>87</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,10 +1244,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>31</v>
+        <v>41</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,10 +1258,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>31</v>
+        <v>89</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,10 +1272,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>15</v>
+        <v>90</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -955,10 +1286,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>34</v>
+        <v>13</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -966,10 +1300,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>35</v>
+        <v>80</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -977,10 +1314,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>36</v>
+        <v>62</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -988,10 +1328,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>36</v>
+        <v>69</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,10 +1342,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>36</v>
+        <v>95</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,10 +1356,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>36</v>
+        <v>97</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,10 +1370,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,10 +1384,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1043,10 +1398,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>41</v>
+        <v>91</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1054,10 +1412,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>42</v>
+        <v>84</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,10 +1426,153 @@
         <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added way to add missing teams to teams spreadsheet
</commit_message>
<xml_diff>
--- a/data/odds.xlsx
+++ b/data/odds.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="130">
   <si>
     <t xml:space="preserve">Index</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t xml:space="preserve">UTSA Roadrunners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miami (OH) RedHawks</t>
   </si>
   <si>
     <t xml:space="preserve">Northwestern Wildcats</t>
@@ -706,11 +709,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="39.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1207,10 +1209,10 @@
         <v>8</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1221,16 +1223,16 @@
         <v>33</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1241,16 +1243,16 @@
         <v>33</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,16 +1263,16 @@
         <v>33</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,10 +1289,10 @@
         <v>8</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1307,10 +1309,10 @@
         <v>8</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,10 +1329,10 @@
         <v>8</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,7 +1352,7 @@
         <v>13</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,16 +1363,16 @@
         <v>33</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1381,16 +1383,16 @@
         <v>33</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1401,16 +1403,16 @@
         <v>33</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1421,16 +1423,16 @@
         <v>33</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1447,7 +1449,7 @@
         <v>8</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>10</v>
@@ -1467,10 +1469,10 @@
         <v>8</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,10 +1489,10 @@
         <v>8</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1507,10 +1509,10 @@
         <v>8</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,19 +1520,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1538,16 +1540,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>9</v>
@@ -1558,7 +1560,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>7</v>
@@ -1570,7 +1572,7 @@
         <v>51</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1578,7 +1580,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>47</v>
@@ -1587,10 +1589,10 @@
         <v>8</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1598,19 +1600,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,10 +1620,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>8</v>
@@ -1638,7 +1640,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>11</v>
@@ -1647,10 +1649,10 @@
         <v>8</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1658,7 +1660,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>7</v>
@@ -1667,7 +1669,7 @@
         <v>8</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>29</v>
@@ -1678,7 +1680,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>47</v>
@@ -1687,7 +1689,7 @@
         <v>8</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>49</v>
@@ -1698,7 +1700,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>47</v>
@@ -1707,10 +1709,10 @@
         <v>8</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1718,7 +1720,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>47</v>
@@ -1727,10 +1729,10 @@
         <v>8</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1738,7 +1740,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>47</v>
@@ -1758,10 +1760,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>8</v>
@@ -1778,16 +1780,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F54" s="0" t="s">
         <v>34</v>
@@ -1798,16 +1800,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>46</v>
@@ -1818,7 +1820,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>47</v>
@@ -1827,10 +1829,10 @@
         <v>8</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1838,10 +1840,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>8</v>
@@ -1858,19 +1860,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,10 +1880,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>8</v>
@@ -1890,7 +1892,7 @@
         <v>24</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1898,10 +1900,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>8</v>
@@ -1910,7 +1912,7 @@
         <v>29</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1918,10 +1920,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>8</v>
@@ -1930,7 +1932,7 @@
         <v>15</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,10 +1940,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>8</v>
@@ -1950,7 +1952,7 @@
         <v>46</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1958,19 +1960,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1978,7 +1980,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>47</v>
@@ -1987,10 +1989,10 @@
         <v>8</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1998,10 +2000,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>8</v>
@@ -2010,7 +2012,7 @@
         <v>35</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2018,19 +2020,19 @@
         <v>65</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2038,10 +2040,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>8</v>
@@ -2058,10 +2060,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>8</v>
@@ -2070,7 +2072,7 @@
         <v>57</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2078,7 +2080,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>47</v>
@@ -2098,10 +2100,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>8</v>
@@ -2118,19 +2120,19 @@
         <v>70</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,10 +2140,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>8</v>
@@ -2150,7 +2152,7 @@
         <v>35</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
odds spreadsheet add chance percent columns
</commit_message>
<xml_diff>
--- a/data/odds.xlsx
+++ b/data/odds.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="266">
   <si>
     <t xml:space="preserve">Index</t>
   </si>
@@ -40,12 +40,18 @@
     <t xml:space="preserve">Spread 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Chance 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Team 2</t>
   </si>
   <si>
     <t xml:space="preserve">Spread 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Chance 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Saturday, August 24</t>
   </si>
   <si>
@@ -61,12 +67,18 @@
     <t xml:space="preserve">-13</t>
   </si>
   <si>
+    <t xml:space="preserve">83.0%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Georgia Tech Yellow Jackets</t>
   </si>
   <si>
     <t xml:space="preserve">+13</t>
   </si>
   <si>
+    <t xml:space="preserve">17.0%</t>
+  </si>
+  <si>
     <t xml:space="preserve">8:00 PM</t>
   </si>
   <si>
@@ -76,12 +88,18 @@
     <t xml:space="preserve">-24.5</t>
   </si>
   <si>
+    <t xml:space="preserve">100.0%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nevada Wolf Pack</t>
   </si>
   <si>
     <t xml:space="preserve">+24.5</t>
   </si>
   <si>
+    <t xml:space="preserve">0.0%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thursday, August 29</t>
   </si>
   <si>
@@ -91,36 +109,54 @@
     <t xml:space="preserve">+2</t>
   </si>
   <si>
+    <t xml:space="preserve">46.6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Minnesota Golden Gophers</t>
   </si>
   <si>
     <t xml:space="preserve">-2</t>
   </si>
   <si>
+    <t xml:space="preserve">53.4%</t>
+  </si>
+  <si>
     <t xml:space="preserve">North Dakota Fighting Hawks</t>
   </si>
   <si>
     <t xml:space="preserve">+8</t>
   </si>
   <si>
+    <t xml:space="preserve">26.2%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Colorado Buffaloes</t>
   </si>
   <si>
     <t xml:space="preserve">-8</t>
   </si>
   <si>
+    <t xml:space="preserve">73.8%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coastal Carolina Chanticleers</t>
   </si>
   <si>
     <t xml:space="preserve">+4.5</t>
   </si>
   <si>
+    <t xml:space="preserve">36.9%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jacksonville State Gamecocks</t>
   </si>
   <si>
     <t xml:space="preserve">-4.5</t>
   </si>
   <si>
+    <t xml:space="preserve">63.1%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Friday, August 30</t>
   </si>
   <si>
@@ -145,12 +181,18 @@
     <t xml:space="preserve">+11.5</t>
   </si>
   <si>
+    <t xml:space="preserve">19.4%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Michigan State Spartans</t>
   </si>
   <si>
     <t xml:space="preserve">-11.5</t>
   </si>
   <si>
+    <t xml:space="preserve">80.6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">9:00 PM</t>
   </si>
   <si>
@@ -169,12 +211,18 @@
     <t xml:space="preserve">-8.5</t>
   </si>
   <si>
+    <t xml:space="preserve">74.6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stanford Cardinal</t>
   </si>
   <si>
     <t xml:space="preserve">+8.5</t>
   </si>
   <si>
+    <t xml:space="preserve">25.4%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Saturday, August 31</t>
   </si>
   <si>
@@ -184,12 +232,18 @@
     <t xml:space="preserve">+13.5</t>
   </si>
   <si>
+    <t xml:space="preserve">16.5%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Georgia Bulldogs</t>
   </si>
   <si>
     <t xml:space="preserve">-13.5</t>
   </si>
   <si>
+    <t xml:space="preserve">83.5%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Virginia Tech Hokies</t>
   </si>
   <si>
@@ -214,12 +268,18 @@
     <t xml:space="preserve">-10.5</t>
   </si>
   <si>
+    <t xml:space="preserve">79.3%</t>
+  </si>
+  <si>
     <t xml:space="preserve">West Virginia Mountaineers</t>
   </si>
   <si>
     <t xml:space="preserve">+10.5</t>
   </si>
   <si>
+    <t xml:space="preserve">20.7%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kent State Golden Flashes</t>
   </si>
   <si>
@@ -241,12 +301,18 @@
     <t xml:space="preserve">+9</t>
   </si>
   <si>
+    <t xml:space="preserve">24.9%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oklahoma State Cowboys</t>
   </si>
   <si>
     <t xml:space="preserve">-9</t>
   </si>
   <si>
+    <t xml:space="preserve">75.1%</t>
+  </si>
+  <si>
     <t xml:space="preserve">3:30 PM</t>
   </si>
   <si>
@@ -256,12 +322,18 @@
     <t xml:space="preserve">-2.5</t>
   </si>
   <si>
+    <t xml:space="preserve">54.3%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Florida Gators</t>
   </si>
   <si>
     <t xml:space="preserve">+2.5</t>
   </si>
   <si>
+    <t xml:space="preserve">45.7%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Colorado State Rams</t>
   </si>
   <si>
@@ -280,12 +352,18 @@
     <t xml:space="preserve">+19.5</t>
   </si>
   <si>
+    <t xml:space="preserve">1.6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indiana Hoosiers</t>
   </si>
   <si>
     <t xml:space="preserve">-19.5</t>
   </si>
   <si>
+    <t xml:space="preserve">98.4%</t>
+  </si>
+  <si>
     <t xml:space="preserve">UTEP Miners</t>
   </si>
   <si>
@@ -316,24 +394,36 @@
     <t xml:space="preserve">-1</t>
   </si>
   <si>
+    <t xml:space="preserve">51.2%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Massachusetts Minutemen</t>
   </si>
   <si>
     <t xml:space="preserve">+1</t>
   </si>
   <si>
+    <t xml:space="preserve">48.8%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ohio Bobcats</t>
   </si>
   <si>
     <t xml:space="preserve">+14.5</t>
   </si>
   <si>
+    <t xml:space="preserve">13.2%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Syracuse Orange</t>
   </si>
   <si>
     <t xml:space="preserve">-14.5</t>
   </si>
   <si>
+    <t xml:space="preserve">86.8%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kennesaw State Owls</t>
   </si>
   <si>
@@ -352,12 +442,18 @@
     <t xml:space="preserve">+3.5</t>
   </si>
   <si>
+    <t xml:space="preserve">39.4%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Northwestern Wildcats</t>
   </si>
   <si>
     <t xml:space="preserve">-3.5</t>
   </si>
   <si>
+    <t xml:space="preserve">60.6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">4:00 PM</t>
   </si>
   <si>
@@ -367,12 +463,18 @@
     <t xml:space="preserve">-10</t>
   </si>
   <si>
+    <t xml:space="preserve">77.4%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Georgia Southern Eagles</t>
   </si>
   <si>
     <t xml:space="preserve">+10</t>
   </si>
   <si>
+    <t xml:space="preserve">22.6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">4:15 PM</t>
   </si>
   <si>
@@ -391,12 +493,18 @@
     <t xml:space="preserve">+7</t>
   </si>
   <si>
+    <t xml:space="preserve">29.7%</t>
+  </si>
+  <si>
     <t xml:space="preserve">South Alabama Jaguars</t>
   </si>
   <si>
     <t xml:space="preserve">-7</t>
   </si>
   <si>
+    <t xml:space="preserve">70.3%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Western Kentucky Hilltoppers</t>
   </si>
   <si>
@@ -415,12 +523,18 @@
     <t xml:space="preserve">+3</t>
   </si>
   <si>
+    <t xml:space="preserve">42.6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Houston Cougars</t>
   </si>
   <si>
     <t xml:space="preserve">-3</t>
   </si>
   <si>
+    <t xml:space="preserve">57.4%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sam Houston Bearkats</t>
   </si>
   <si>
@@ -430,12 +544,18 @@
     <t xml:space="preserve">+15.5</t>
   </si>
   <si>
+    <t xml:space="preserve">11.9%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Troy Trojans</t>
   </si>
   <si>
     <t xml:space="preserve">-15.5</t>
   </si>
   <si>
+    <t xml:space="preserve">88.1%</t>
+  </si>
+  <si>
     <t xml:space="preserve">7:30 PM</t>
   </si>
   <si>
@@ -520,12 +640,18 @@
     <t xml:space="preserve">+6</t>
   </si>
   <si>
+    <t xml:space="preserve">33.6%</t>
+  </si>
+  <si>
     <t xml:space="preserve">LSU Tigers</t>
   </si>
   <si>
     <t xml:space="preserve">-6</t>
   </si>
   <si>
+    <t xml:space="preserve">66.4%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Monday, September 2</t>
   </si>
   <si>
@@ -556,21 +682,33 @@
     <t xml:space="preserve">+6.5</t>
   </si>
   <si>
+    <t xml:space="preserve">32.3%</t>
+  </si>
+  <si>
     <t xml:space="preserve">-6.5</t>
   </si>
   <si>
+    <t xml:space="preserve">67.7%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Friday, September 13</t>
   </si>
   <si>
     <t xml:space="preserve">+7.5</t>
   </si>
   <si>
+    <t xml:space="preserve">27.0%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kansas State Wildcats</t>
   </si>
   <si>
     <t xml:space="preserve">-7.5</t>
   </si>
   <si>
+    <t xml:space="preserve">73.0%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Saturday, September 14</t>
   </si>
   <si>
@@ -598,15 +736,27 @@
     <t xml:space="preserve">-1.5</t>
   </si>
   <si>
+    <t xml:space="preserve">52.5%</t>
+  </si>
+  <si>
     <t xml:space="preserve">+1.5</t>
   </si>
   <si>
+    <t xml:space="preserve">47.5%</t>
+  </si>
+  <si>
     <t xml:space="preserve">+9.5</t>
   </si>
   <si>
+    <t xml:space="preserve">24.5%</t>
+  </si>
+  <si>
     <t xml:space="preserve">-9.5</t>
   </si>
   <si>
+    <t xml:space="preserve">75.5%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Friday, September 27</t>
   </si>
   <si>
@@ -622,9 +772,15 @@
     <t xml:space="preserve">+5.5</t>
   </si>
   <si>
+    <t xml:space="preserve">34.9%</t>
+  </si>
+  <si>
     <t xml:space="preserve">-5.5</t>
   </si>
   <si>
+    <t xml:space="preserve">65.1%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Duke Blue Devils</t>
   </si>
   <si>
@@ -637,13 +793,22 @@
     <t xml:space="preserve">+4</t>
   </si>
   <si>
+    <t xml:space="preserve">38.1%</t>
+  </si>
+  <si>
     <t xml:space="preserve">-4</t>
   </si>
   <si>
+    <t xml:space="preserve">61.9%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Saturday, October 12</t>
   </si>
   <si>
     <t xml:space="preserve">-0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50.0%</t>
   </si>
   <si>
     <t xml:space="preserve">Saturday, October 19</t>
@@ -944,7 +1109,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -952,10 +1117,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -983,31 +1149,43 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,25 +1193,31 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,25 +1225,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1067,25 +1257,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>28</v>
+        <v>36</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,25 +1289,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1119,25 +1321,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>38</v>
+        <v>49</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,25 +1353,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>42</v>
+        <v>54</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1171,25 +1385,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>17</v>
+        <v>59</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1197,25 +1417,31 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>50</v>
+        <v>64</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1223,25 +1449,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>55</v>
+        <v>71</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1249,25 +1481,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>53</v>
+        <v>75</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1275,25 +1513,31 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>61</v>
+        <v>78</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,25 +1545,31 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>65</v>
+        <v>83</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,25 +1577,31 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>69</v>
+        <v>88</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1353,25 +1609,31 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>74</v>
+        <v>94</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1379,25 +1641,31 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>79</v>
+        <v>101</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1405,25 +1673,31 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>83</v>
+        <v>106</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1431,25 +1705,31 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>87</v>
+        <v>111</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1457,25 +1737,31 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>91</v>
+        <v>116</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1483,25 +1769,31 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>94</v>
+        <v>25</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>95</v>
+        <v>120</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,25 +1801,31 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>99</v>
+        <v>125</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,25 +1833,31 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>103</v>
+        <v>131</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1561,25 +1865,31 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>107</v>
+        <v>136</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,25 +1897,31 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>111</v>
+        <v>141</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,25 +1929,31 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>116</v>
+        <v>148</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1639,25 +1961,31 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>61</v>
+        <v>153</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,25 +1993,31 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>124</v>
+        <v>158</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1691,25 +2025,31 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>127</v>
+        <v>25</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>128</v>
+        <v>163</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,25 +2057,31 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>130</v>
+        <v>166</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>132</v>
+        <v>168</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1743,25 +2089,31 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>134</v>
+        <v>53</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>42</v>
+        <v>172</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1769,25 +2121,31 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>137</v>
+        <v>175</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,25 +2153,31 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>97</v>
+        <v>180</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1821,25 +2185,31 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>141</v>
+        <v>181</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>142</v>
+        <v>182</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>143</v>
+        <v>25</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>144</v>
+        <v>183</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1847,25 +2217,31 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>146</v>
+        <v>73</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>53</v>
+        <v>186</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1873,25 +2249,31 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>148</v>
+        <v>188</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>149</v>
+        <v>189</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>150</v>
+        <v>25</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>151</v>
+        <v>190</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1899,25 +2281,31 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>152</v>
+        <v>192</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>153</v>
+        <v>193</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>154</v>
+        <v>16</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1925,25 +2313,31 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>155</v>
+        <v>195</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>72</v>
+        <v>196</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1951,25 +2345,31 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>157</v>
+        <v>197</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>158</v>
+        <v>198</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>159</v>
+        <v>25</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>160</v>
+        <v>199</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1977,25 +2377,31 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>161</v>
+        <v>201</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>124</v>
+        <v>202</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2003,25 +2409,31 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>163</v>
+        <v>203</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>164</v>
+        <v>204</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>165</v>
+        <v>205</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>167</v>
+        <v>207</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2029,25 +2441,31 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>169</v>
+        <v>211</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>170</v>
+        <v>212</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>171</v>
+        <v>13</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2055,25 +2473,31 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="G43" s="0" t="s">
         <v>143</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>109</v>
+        <v>183</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2081,25 +2505,31 @@
         <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>173</v>
+        <v>215</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>77</v>
+        <v>216</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2107,25 +2537,31 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>175</v>
+        <v>217</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>176</v>
+        <v>44</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>30</v>
+        <v>218</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,25 +2569,31 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>177</v>
+        <v>219</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>90</v>
+        <v>220</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>178</v>
+        <v>116</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2159,25 +2601,31 @@
         <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>182</v>
+        <v>226</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2185,25 +2633,31 @@
         <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>183</v>
+        <v>229</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>50</v>
+        <v>59</v>
+      </c>
+      <c r="I48" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2211,25 +2665,31 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>183</v>
+        <v>229</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E49" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="J49" s="0" t="s">
         <v>140</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G49" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H49" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2237,25 +2697,31 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>183</v>
+        <v>229</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>184</v>
+        <v>230</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>154</v>
+        <v>194</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>185</v>
+        <v>22</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>153</v>
+        <v>231</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2263,25 +2729,31 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>183</v>
+        <v>229</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>186</v>
+        <v>232</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>187</v>
+        <v>66</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>48</v>
+        <v>233</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2289,25 +2761,31 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>183</v>
+        <v>229</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>30</v>
+        <v>88</v>
+      </c>
+      <c r="I52" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2315,25 +2793,31 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>183</v>
+        <v>229</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>182</v>
+        <v>227</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>80</v>
+        <v>228</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>180</v>
+        <v>104</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,25 +2825,31 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>188</v>
+        <v>234</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>52</v>
+        <v>157</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>74</v>
+        <v>68</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2367,25 +2857,31 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>188</v>
+        <v>234</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>190</v>
+        <v>236</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>73</v>
+        <v>238</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>192</v>
+        <v>94</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2393,25 +2889,31 @@
         <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>188</v>
+        <v>234</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>164</v>
+        <v>204</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>193</v>
+        <v>241</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>143</v>
+        <v>242</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>194</v>
+        <v>183</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2419,25 +2921,31 @@
         <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>76</v>
+        <v>225</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>182</v>
+        <v>98</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2445,25 +2953,31 @@
         <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>197</v>
+        <v>247</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>140</v>
+        <v>85</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>63</v>
+        <v>180</v>
+      </c>
+      <c r="I58" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="J58" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2471,25 +2985,31 @@
         <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>198</v>
+        <v>100</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>79</v>
+        <v>248</v>
+      </c>
+      <c r="I59" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2497,25 +3017,31 @@
         <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>199</v>
+        <v>249</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>164</v>
+        <v>250</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
+      </c>
+      <c r="I60" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="J60" s="0" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2523,25 +3049,31 @@
         <v>60</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>201</v>
+        <v>170</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>130</v>
+        <v>253</v>
+      </c>
+      <c r="I61" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="J61" s="0" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2549,25 +3081,31 @@
         <v>61</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>199</v>
+        <v>249</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>181</v>
+        <v>250</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>200</v>
+        <v>226</v>
+      </c>
+      <c r="I62" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="J62" s="0" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2575,25 +3113,31 @@
         <v>62</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>193</v>
+        <v>241</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>190</v>
+        <v>242</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>194</v>
+        <v>236</v>
+      </c>
+      <c r="I63" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2601,25 +3145,31 @@
         <v>63</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>202</v>
+        <v>254</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>193</v>
+        <v>241</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>139</v>
+        <v>242</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>194</v>
+        <v>179</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2627,25 +3177,31 @@
         <v>64</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>127</v>
+        <v>44</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>109</v>
+        <v>163</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2653,25 +3209,31 @@
         <v>65</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>203</v>
+        <v>255</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>187</v>
+        <v>96</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>72</v>
+        <v>233</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2679,25 +3241,31 @@
         <v>66</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>203</v>
+        <v>255</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>204</v>
+        <v>256</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>11</v>
+        <v>257</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>205</v>
+        <v>13</v>
+      </c>
+      <c r="I67" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="J67" s="0" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2705,25 +3273,31 @@
         <v>67</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>206</v>
+        <v>260</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>184</v>
+        <v>127</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>207</v>
+        <v>230</v>
+      </c>
+      <c r="I68" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="J68" s="0" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2731,25 +3305,31 @@
         <v>68</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>206</v>
+        <v>260</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>193</v>
+        <v>49</v>
+      </c>
+      <c r="I69" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2757,25 +3337,31 @@
         <v>69</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>208</v>
+        <v>263</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>82</v>
+        <v>238</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>207</v>
+        <v>106</v>
+      </c>
+      <c r="I70" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="J70" s="0" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2783,25 +3369,31 @@
         <v>70</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>209</v>
+        <v>264</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>166</v>
+        <v>103</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>77</v>
+        <v>207</v>
+      </c>
+      <c r="I71" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J71" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2809,25 +3401,31 @@
         <v>71</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>209</v>
+        <v>264</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>178</v>
+        <v>221</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>177</v>
+        <v>265</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="J72" s="0" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created json files in their own directory
</commit_message>
<xml_diff>
--- a/data/odds.xlsx
+++ b/data/odds.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="268">
   <si>
     <t>Index</t>
   </si>
@@ -316,7 +316,7 @@
     <t>Michigan Wolverines</t>
   </si>
   <si>
-    <t>East Tennessee State Buccaneers</t>
+    <t>Ohio State Buckeyes</t>
   </si>
   <si>
     <t>-13</t>
@@ -349,126 +349,126 @@
     <t>+13.5</t>
   </si>
   <si>
+    <t>+21</t>
+  </si>
+  <si>
+    <t>-10.5</t>
+  </si>
+  <si>
+    <t>+23.5</t>
+  </si>
+  <si>
+    <t>+9</t>
+  </si>
+  <si>
+    <t>-2.5</t>
+  </si>
+  <si>
+    <t>+36.5</t>
+  </si>
+  <si>
+    <t>+19.5</t>
+  </si>
+  <si>
+    <t>+28</t>
+  </si>
+  <si>
+    <t>+50.5</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>+14.5</t>
+  </si>
+  <si>
+    <t>+22.5</t>
+  </si>
+  <si>
+    <t>+3.5</t>
+  </si>
+  <si>
+    <t>-10</t>
+  </si>
+  <si>
+    <t>+7</t>
+  </si>
+  <si>
+    <t>+31</t>
+  </si>
+  <si>
+    <t>+3</t>
+  </si>
+  <si>
+    <t>+12</t>
+  </si>
+  <si>
+    <t>+15.5</t>
+  </si>
+  <si>
+    <t>+1</t>
+  </si>
+  <si>
+    <t>+20.5</t>
+  </si>
+  <si>
     <t>-13.5</t>
   </si>
   <si>
-    <t>+21</t>
-  </si>
-  <si>
-    <t>-10.5</t>
-  </si>
-  <si>
-    <t>+23.5</t>
-  </si>
-  <si>
-    <t>+9</t>
-  </si>
-  <si>
-    <t>-2.5</t>
-  </si>
-  <si>
-    <t>+36</t>
-  </si>
-  <si>
-    <t>+19.5</t>
-  </si>
-  <si>
-    <t>+28</t>
-  </si>
-  <si>
-    <t>+50.5</t>
-  </si>
-  <si>
-    <t>-1</t>
-  </si>
-  <si>
-    <t>+14.5</t>
-  </si>
-  <si>
-    <t>+22.5</t>
-  </si>
-  <si>
-    <t>+3.5</t>
-  </si>
-  <si>
-    <t>-10</t>
-  </si>
-  <si>
-    <t>+7</t>
-  </si>
-  <si>
-    <t>+31</t>
-  </si>
-  <si>
-    <t>+3</t>
-  </si>
-  <si>
-    <t>+15.5</t>
-  </si>
-  <si>
-    <t>+1</t>
-  </si>
-  <si>
-    <t>+20</t>
-  </si>
-  <si>
     <t>+25.5</t>
   </si>
   <si>
-    <t>+20.5</t>
+    <t>+30.5</t>
+  </si>
+  <si>
+    <t>+6</t>
+  </si>
+  <si>
+    <t>+22</t>
+  </si>
+  <si>
+    <t>-3.5</t>
+  </si>
+  <si>
+    <t>+2.5</t>
+  </si>
+  <si>
+    <t>-4.5</t>
+  </si>
+  <si>
+    <t>+6.5</t>
+  </si>
+  <si>
+    <t>+7.5</t>
+  </si>
+  <si>
+    <t>-20.5</t>
+  </si>
+  <si>
+    <t>+8.5</t>
+  </si>
+  <si>
+    <t>-7.5</t>
+  </si>
+  <si>
+    <t>-1.5</t>
+  </si>
+  <si>
+    <t>+10.5</t>
+  </si>
+  <si>
+    <t>+5.5</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>+9.5</t>
   </si>
   <si>
     <t>-9</t>
   </si>
   <si>
-    <t>+30.5</t>
-  </si>
-  <si>
-    <t>+6</t>
-  </si>
-  <si>
-    <t>+22</t>
-  </si>
-  <si>
-    <t>-3.5</t>
-  </si>
-  <si>
-    <t>+2.5</t>
-  </si>
-  <si>
-    <t>-4.5</t>
-  </si>
-  <si>
-    <t>+6.5</t>
-  </si>
-  <si>
-    <t>+7.5</t>
-  </si>
-  <si>
-    <t>-20.5</t>
-  </si>
-  <si>
-    <t>+8.5</t>
-  </si>
-  <si>
-    <t>-7.5</t>
-  </si>
-  <si>
-    <t>-1.5</t>
-  </si>
-  <si>
-    <t>+9.5</t>
-  </si>
-  <si>
-    <t>+10.5</t>
-  </si>
-  <si>
-    <t>+5.5</t>
-  </si>
-  <si>
-    <t>-3</t>
-  </si>
-  <si>
     <t>+4</t>
   </si>
   <si>
@@ -502,87 +502,90 @@
     <t>16.5%</t>
   </si>
   <si>
+    <t>79.3%</t>
+  </si>
+  <si>
+    <t>24.9%</t>
+  </si>
+  <si>
+    <t>54.3%</t>
+  </si>
+  <si>
+    <t>1.6%</t>
+  </si>
+  <si>
+    <t>51.2%</t>
+  </si>
+  <si>
+    <t>13.2%</t>
+  </si>
+  <si>
+    <t>39.4%</t>
+  </si>
+  <si>
+    <t>77.4%</t>
+  </si>
+  <si>
+    <t>29.7%</t>
+  </si>
+  <si>
+    <t>42.6%</t>
+  </si>
+  <si>
+    <t>18.4%</t>
+  </si>
+  <si>
+    <t>11.9%</t>
+  </si>
+  <si>
+    <t>48.8%</t>
+  </si>
+  <si>
     <t>83.5%</t>
   </si>
   <si>
-    <t>79.3%</t>
-  </si>
-  <si>
-    <t>24.9%</t>
-  </si>
-  <si>
-    <t>54.3%</t>
-  </si>
-  <si>
-    <t>1.6%</t>
-  </si>
-  <si>
-    <t>51.2%</t>
-  </si>
-  <si>
-    <t>13.2%</t>
-  </si>
-  <si>
-    <t>39.4%</t>
-  </si>
-  <si>
-    <t>77.4%</t>
-  </si>
-  <si>
-    <t>29.7%</t>
-  </si>
-  <si>
-    <t>42.6%</t>
-  </si>
-  <si>
-    <t>11.9%</t>
-  </si>
-  <si>
-    <t>48.8%</t>
+    <t>33.6%</t>
+  </si>
+  <si>
+    <t>60.6%</t>
+  </si>
+  <si>
+    <t>45.7%</t>
+  </si>
+  <si>
+    <t>63.1%</t>
+  </si>
+  <si>
+    <t>32.3%</t>
+  </si>
+  <si>
+    <t>27.0%</t>
+  </si>
+  <si>
+    <t>25.4%</t>
+  </si>
+  <si>
+    <t>73.0%</t>
+  </si>
+  <si>
+    <t>52.5%</t>
+  </si>
+  <si>
+    <t>20.7%</t>
+  </si>
+  <si>
+    <t>34.9%</t>
+  </si>
+  <si>
+    <t>57.4%</t>
+  </si>
+  <si>
+    <t>24.5%</t>
   </si>
   <si>
     <t>75.1%</t>
   </si>
   <si>
-    <t>33.6%</t>
-  </si>
-  <si>
-    <t>60.6%</t>
-  </si>
-  <si>
-    <t>45.7%</t>
-  </si>
-  <si>
-    <t>63.1%</t>
-  </si>
-  <si>
-    <t>32.3%</t>
-  </si>
-  <si>
-    <t>27.0%</t>
-  </si>
-  <si>
-    <t>25.4%</t>
-  </si>
-  <si>
-    <t>73.0%</t>
-  </si>
-  <si>
-    <t>52.5%</t>
-  </si>
-  <si>
-    <t>24.5%</t>
-  </si>
-  <si>
-    <t>20.7%</t>
-  </si>
-  <si>
-    <t>34.9%</t>
-  </si>
-  <si>
-    <t>57.4%</t>
-  </si>
-  <si>
     <t>38.1%</t>
   </si>
   <si>
@@ -709,7 +712,7 @@
     <t>-23.5</t>
   </si>
   <si>
-    <t>-36</t>
+    <t>-36.5</t>
   </si>
   <si>
     <t>-19.5</t>
@@ -736,12 +739,12 @@
     <t>-31</t>
   </si>
   <si>
+    <t>-12</t>
+  </si>
+  <si>
     <t>-15.5</t>
   </si>
   <si>
-    <t>-20</t>
-  </si>
-  <si>
     <t>-25.5</t>
   </si>
   <si>
@@ -757,12 +760,12 @@
     <t>+1.5</t>
   </si>
   <si>
+    <t>-5.5</t>
+  </si>
+  <si>
     <t>-9.5</t>
   </si>
   <si>
-    <t>-5.5</t>
-  </si>
-  <si>
     <t>-4</t>
   </si>
   <si>
@@ -793,6 +796,9 @@
     <t>70.3%</t>
   </si>
   <si>
+    <t>81.6%</t>
+  </si>
+  <si>
     <t>88.1%</t>
   </si>
   <si>
@@ -802,10 +808,10 @@
     <t>47.5%</t>
   </si>
   <si>
+    <t>65.1%</t>
+  </si>
+  <si>
     <t>75.5%</t>
-  </si>
-  <si>
-    <t>65.1%</t>
   </si>
   <si>
     <t>61.9%</t>
@@ -1230,13 +1236,13 @@
         <v>153</v>
       </c>
       <c r="H2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1294,13 +1300,13 @@
         <v>155</v>
       </c>
       <c r="H4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1329,10 +1335,10 @@
         <v>84</v>
       </c>
       <c r="I5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="J5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1358,10 +1364,10 @@
         <v>157</v>
       </c>
       <c r="H6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J6" t="s">
         <v>179</v>
@@ -1393,7 +1399,7 @@
         <v>94</v>
       </c>
       <c r="I7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="J7" t="s">
         <v>154</v>
@@ -1422,13 +1428,13 @@
         <v>159</v>
       </c>
       <c r="H8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I8" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="J8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1486,10 +1492,10 @@
         <v>160</v>
       </c>
       <c r="H10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J10" t="s">
         <v>182</v>
@@ -1521,10 +1527,10 @@
         <v>98</v>
       </c>
       <c r="I11" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="J11" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1544,19 +1550,19 @@
         <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="G12" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="H12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I12" t="s">
-        <v>110</v>
+        <v>225</v>
       </c>
       <c r="J12" t="s">
-        <v>161</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1576,16 +1582,16 @@
         <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G13" t="s">
         <v>158</v>
       </c>
       <c r="H13" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I13" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J13" t="s">
         <v>154</v>
@@ -1608,19 +1614,19 @@
         <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H14" t="s">
         <v>90</v>
       </c>
       <c r="I14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1640,16 +1646,16 @@
         <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G15" t="s">
         <v>158</v>
       </c>
       <c r="H15" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I15" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="J15" t="s">
         <v>154</v>
@@ -1672,19 +1678,19 @@
         <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H16" t="s">
         <v>96</v>
       </c>
       <c r="I16" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="J16" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1704,16 +1710,16 @@
         <v>55</v>
       </c>
       <c r="F17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H17" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J17" t="s">
         <v>178</v>
@@ -1736,7 +1742,7 @@
         <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G18" t="s">
         <v>158</v>
@@ -1745,7 +1751,7 @@
         <v>81</v>
       </c>
       <c r="I18" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="J18" t="s">
         <v>154</v>
@@ -1768,19 +1774,19 @@
         <v>57</v>
       </c>
       <c r="F19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I19" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="J19" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1800,16 +1806,16 @@
         <v>58</v>
       </c>
       <c r="F20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G20" t="s">
         <v>158</v>
       </c>
       <c r="H20" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I20" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="J20" t="s">
         <v>154</v>
@@ -1832,7 +1838,7 @@
         <v>59</v>
       </c>
       <c r="F21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G21" t="s">
         <v>158</v>
@@ -1841,7 +1847,7 @@
         <v>100</v>
       </c>
       <c r="I21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J21" t="s">
         <v>154</v>
@@ -1864,13 +1870,13 @@
         <v>60</v>
       </c>
       <c r="F22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H22" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I22" t="s">
         <v>130</v>
@@ -1896,19 +1902,19 @@
         <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H23" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I23" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="J23" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1928,16 +1934,16 @@
         <v>62</v>
       </c>
       <c r="F24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G24" t="s">
         <v>158</v>
       </c>
       <c r="H24" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I24" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="J24" t="s">
         <v>154</v>
@@ -1960,16 +1966,16 @@
         <v>63</v>
       </c>
       <c r="F25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H25" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J25" t="s">
         <v>177</v>
@@ -1992,19 +1998,19 @@
         <v>64</v>
       </c>
       <c r="F26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H26" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I26" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="J26" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2024,16 +2030,16 @@
         <v>65</v>
       </c>
       <c r="F27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G27" t="s">
         <v>158</v>
       </c>
       <c r="H27" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J27" t="s">
         <v>154</v>
@@ -2056,19 +2062,19 @@
         <v>66</v>
       </c>
       <c r="F28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H28" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I28" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J28" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2088,7 +2094,7 @@
         <v>67</v>
       </c>
       <c r="F29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G29" t="s">
         <v>158</v>
@@ -2097,7 +2103,7 @@
         <v>86</v>
       </c>
       <c r="I29" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="J29" t="s">
         <v>154</v>
@@ -2120,19 +2126,19 @@
         <v>68</v>
       </c>
       <c r="F30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2152,19 +2158,19 @@
         <v>69</v>
       </c>
       <c r="F31" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="G31" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="H31" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I31" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="J31" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2190,13 +2196,13 @@
         <v>173</v>
       </c>
       <c r="H32" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I32" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="J32" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2225,10 +2231,10 @@
         <v>87</v>
       </c>
       <c r="I33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2257,7 +2263,7 @@
         <v>99</v>
       </c>
       <c r="I34" t="s">
-        <v>241</v>
+        <v>142</v>
       </c>
       <c r="J34" t="s">
         <v>154</v>
@@ -2280,13 +2286,13 @@
         <v>73</v>
       </c>
       <c r="F35" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="G35" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="H35" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I35" t="s">
         <v>110</v>
@@ -2312,16 +2318,16 @@
         <v>74</v>
       </c>
       <c r="F36" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G36" t="s">
         <v>158</v>
       </c>
       <c r="H36" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I36" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="J36" t="s">
         <v>154</v>
@@ -2344,16 +2350,16 @@
         <v>75</v>
       </c>
       <c r="F37" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G37" t="s">
         <v>158</v>
       </c>
       <c r="H37" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J37" t="s">
         <v>154</v>
@@ -2376,19 +2382,19 @@
         <v>76</v>
       </c>
       <c r="F38" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="G38" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="H38" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I38" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="J38" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2408,7 +2414,7 @@
         <v>77</v>
       </c>
       <c r="F39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G39" t="s">
         <v>158</v>
@@ -2417,7 +2423,7 @@
         <v>85</v>
       </c>
       <c r="I39" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="J39" t="s">
         <v>154</v>
@@ -2440,19 +2446,19 @@
         <v>78</v>
       </c>
       <c r="F40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H40" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I40" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J40" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2472,19 +2478,19 @@
         <v>79</v>
       </c>
       <c r="F41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G41" t="s">
         <v>176</v>
       </c>
       <c r="H41" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I41" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="J41" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2504,7 +2510,7 @@
         <v>80</v>
       </c>
       <c r="F42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G42" t="s">
         <v>158</v>
@@ -2513,7 +2519,7 @@
         <v>40</v>
       </c>
       <c r="I42" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J42" t="s">
         <v>154</v>
@@ -2536,7 +2542,7 @@
         <v>81</v>
       </c>
       <c r="F43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G43" t="s">
         <v>177</v>
@@ -2545,10 +2551,10 @@
         <v>99</v>
       </c>
       <c r="I43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2568,19 +2574,19 @@
         <v>82</v>
       </c>
       <c r="F44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G44" t="s">
         <v>178</v>
       </c>
       <c r="H44" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J44" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2600,7 +2606,7 @@
         <v>83</v>
       </c>
       <c r="F45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G45" t="s">
         <v>179</v>
@@ -2632,19 +2638,19 @@
         <v>84</v>
       </c>
       <c r="F46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G46" t="s">
         <v>180</v>
       </c>
       <c r="H46" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I46" t="s">
         <v>152</v>
       </c>
       <c r="J46" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2664,16 +2670,16 @@
         <v>85</v>
       </c>
       <c r="F47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G47" t="s">
         <v>181</v>
       </c>
       <c r="H47" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J47" t="s">
         <v>183</v>
@@ -2705,7 +2711,7 @@
         <v>95</v>
       </c>
       <c r="I48" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J48" t="s">
         <v>182</v>
@@ -2728,19 +2734,19 @@
         <v>87</v>
       </c>
       <c r="F49" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G49" t="s">
         <v>177</v>
       </c>
       <c r="H49" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I49" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2760,16 +2766,16 @@
         <v>88</v>
       </c>
       <c r="F50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G50" t="s">
         <v>154</v>
       </c>
       <c r="H50" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I50" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J50" t="s">
         <v>158</v>
@@ -2792,13 +2798,13 @@
         <v>89</v>
       </c>
       <c r="F51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G51" t="s">
         <v>182</v>
       </c>
       <c r="H51" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I51" t="s">
         <v>109</v>
@@ -2824,13 +2830,13 @@
         <v>90</v>
       </c>
       <c r="F52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G52" t="s">
         <v>179</v>
       </c>
       <c r="H52" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I52" t="s">
         <v>105</v>
@@ -2856,7 +2862,7 @@
         <v>84</v>
       </c>
       <c r="F53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G53" t="s">
         <v>183</v>
@@ -2865,7 +2871,7 @@
         <v>56</v>
       </c>
       <c r="I53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J53" t="s">
         <v>181</v>
@@ -2888,19 +2894,19 @@
         <v>91</v>
       </c>
       <c r="F54" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H54" t="s">
         <v>49</v>
       </c>
       <c r="I54" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="J54" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2920,7 +2926,7 @@
         <v>92</v>
       </c>
       <c r="F55" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G55" t="s">
         <v>184</v>
@@ -2929,10 +2935,10 @@
         <v>96</v>
       </c>
       <c r="I55" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="J55" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2952,19 +2958,19 @@
         <v>79</v>
       </c>
       <c r="F56" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G56" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H56" t="s">
         <v>99</v>
       </c>
       <c r="I56" t="s">
-        <v>247</v>
+        <v>109</v>
       </c>
       <c r="J56" t="s">
-        <v>262</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2984,7 +2990,7 @@
         <v>50</v>
       </c>
       <c r="F57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G57" t="s">
         <v>181</v>
@@ -2993,7 +2999,7 @@
         <v>55</v>
       </c>
       <c r="I57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J57" t="s">
         <v>183</v>
@@ -3016,19 +3022,19 @@
         <v>93</v>
       </c>
       <c r="F58" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G58" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H58" t="s">
         <v>87</v>
       </c>
       <c r="I58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -3048,16 +3054,16 @@
         <v>94</v>
       </c>
       <c r="F59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G59" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H59" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I59" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J59" t="s">
         <v>178</v>
@@ -3080,10 +3086,10 @@
         <v>95</v>
       </c>
       <c r="F60" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G60" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H60" t="s">
         <v>79</v>
@@ -3092,7 +3098,7 @@
         <v>248</v>
       </c>
       <c r="J60" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -3112,19 +3118,19 @@
         <v>42</v>
       </c>
       <c r="F61" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G61" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H61" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I61" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J61" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -3144,19 +3150,19 @@
         <v>96</v>
       </c>
       <c r="F62" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G62" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H62" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I62" t="s">
         <v>248</v>
       </c>
       <c r="J62" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -3176,19 +3182,19 @@
         <v>85</v>
       </c>
       <c r="F63" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G63" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="H63" t="s">
         <v>92</v>
       </c>
       <c r="I63" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="J63" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -3208,19 +3214,19 @@
         <v>97</v>
       </c>
       <c r="F64" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G64" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="H64" t="s">
         <v>71</v>
       </c>
       <c r="I64" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="J64" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -3240,7 +3246,7 @@
         <v>98</v>
       </c>
       <c r="F65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G65" t="s">
         <v>179</v>
@@ -3249,10 +3255,10 @@
         <v>86</v>
       </c>
       <c r="I65" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -3272,19 +3278,19 @@
         <v>99</v>
       </c>
       <c r="F66" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="G66" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="H66" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I66" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J66" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -3307,16 +3313,16 @@
         <v>151</v>
       </c>
       <c r="G67" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H67" t="s">
         <v>40</v>
       </c>
       <c r="I67" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="J67" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -3345,10 +3351,10 @@
         <v>88</v>
       </c>
       <c r="I68" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="J68" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -3377,10 +3383,10 @@
         <v>94</v>
       </c>
       <c r="I69" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="J69" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -3400,7 +3406,7 @@
         <v>98</v>
       </c>
       <c r="F70" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G70" t="s">
         <v>184</v>
@@ -3409,10 +3415,10 @@
         <v>81</v>
       </c>
       <c r="I70" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="J70" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -3432,19 +3438,19 @@
         <v>86</v>
       </c>
       <c r="F71" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G71" t="s">
         <v>178</v>
       </c>
       <c r="H71" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I71" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J71" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -3467,13 +3473,13 @@
         <v>152</v>
       </c>
       <c r="G72" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H72" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I72" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J72" t="s">
         <v>180</v>

</xml_diff>